<commit_message>
Rank, Logo, Footer fixed
</commit_message>
<xml_diff>
--- a/static/files/student.xlsx
+++ b/static/files/student.xlsx
@@ -97,52 +97,52 @@
     <t>32</t>
   </si>
   <si>
+    <t>Ravinder</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>fghij</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>vkrishr.teja@gmail.com</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>92.6</t>
+  </si>
+  <si>
+    <t>blah blah</t>
+  </si>
+  <si>
+    <t>blah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>GH@GGJ.VOM</t>
+  </si>
+  <si>
+    <t>djkk</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>blah@gmail.com</t>
+  </si>
+  <si>
+    <t>yyuuyyuu</t>
+  </si>
+  <si>
     <t>griet</t>
-  </si>
-  <si>
-    <t>Ravinder</t>
-  </si>
-  <si>
-    <t>abcde</t>
-  </si>
-  <si>
-    <t>fghij</t>
-  </si>
-  <si>
-    <t>Haryana</t>
-  </si>
-  <si>
-    <t>vkrishr.teja@gmail.com</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>92.6</t>
-  </si>
-  <si>
-    <t>blah blah</t>
-  </si>
-  <si>
-    <t>blah</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>GH@GGJ.VOM</t>
-  </si>
-  <si>
-    <t>djkk</t>
-  </si>
-  <si>
-    <t>Andhra Pradesh</t>
-  </si>
-  <si>
-    <t>blah@gmail.com</t>
-  </si>
-  <si>
-    <t>yyuuyyuu</t>
   </si>
   <si>
     <t>hi@hi.com</t>
@@ -625,37 +625,35 @@
       <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
+      <c r="J2" t="s"/>
       <c r="K2" t="n">
         <v>999999999</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s"/>
       <c r="N2" t="s"/>
       <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>30</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
       </c>
       <c r="R2" t="n">
         <v>55555</v>
       </c>
       <c r="S2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" t="s">
         <v>32</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>33</v>
-      </c>
-      <c r="U2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -666,14 +664,14 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
       </c>
       <c r="E3" t="s"/>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s"/>
       <c r="H3" t="s"/>
@@ -686,22 +684,22 @@
       <c r="M3" t="s"/>
       <c r="N3" t="s"/>
       <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
         <v>38</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>39</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>40</v>
       </c>
       <c r="R3" t="n">
         <v>6666666</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U3" t="s"/>
     </row>
@@ -713,17 +711,19 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s"/>
       <c r="H4" t="s"/>
       <c r="I4" t="s"/>
-      <c r="J4" t="s"/>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
       <c r="M4" t="s"/>
@@ -731,7 +731,7 @@
       <c r="O4" t="s"/>
       <c r="P4" t="s"/>
       <c r="Q4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R4" t="s"/>
       <c r="S4" t="s">
@@ -757,7 +757,7 @@
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s"/>
       <c r="H5" t="s"/>
@@ -770,7 +770,7 @@
       <c r="O5" t="s"/>
       <c r="P5" t="s"/>
       <c r="Q5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R5" t="s"/>
       <c r="S5" t="s"/>
@@ -792,14 +792,12 @@
       </c>
       <c r="E6" t="s"/>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s"/>
       <c r="H6" t="s"/>
       <c r="I6" t="s"/>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
+      <c r="J6" t="s"/>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
       <c r="M6" t="s"/>
@@ -807,7 +805,7 @@
       <c r="O6" t="s"/>
       <c r="P6" t="s"/>
       <c r="Q6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R6" t="s"/>
       <c r="S6" t="s">
@@ -835,7 +833,7 @@
         <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s"/>
       <c r="H7" t="s"/>
@@ -848,7 +846,7 @@
       <c r="O7" t="s"/>
       <c r="P7" t="s"/>
       <c r="Q7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R7" t="s"/>
       <c r="S7" t="s">

</xml_diff>